<commit_message>
consideration of ux value
</commit_message>
<xml_diff>
--- a/literature/05.primary-experiment/分析結果.xlsx
+++ b/literature/05.primary-experiment/分析結果.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="探索" sheetId="1" r:id="rId1"/>
@@ -14032,16 +14032,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19998,8 +19998,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AP102"/>
   <sheetViews>
-    <sheetView topLeftCell="AG6" workbookViewId="0">
-      <selection activeCell="AM32" sqref="AM32"/>
+    <sheetView tabSelected="1" topLeftCell="AK6" workbookViewId="0">
+      <selection activeCell="AT34" sqref="AT34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -26891,7 +26891,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:Y59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="L17" workbookViewId="0">
       <selection activeCell="K24" sqref="J19:K24"/>
     </sheetView>
   </sheetViews>

</xml_diff>